<commit_message>
mainPCAstatic aangepast met goede test-train- validate splits.
</commit_message>
<xml_diff>
--- a/results_PCAstatic_with_AIC_BIC_AdjustedR2_LogLikelihood_Residuals.xlsx
+++ b/results_PCAstatic_with_AIC_BIC_AdjustedR2_LogLikelihood_Residuals.xlsx
@@ -456,17 +456,17 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>RMSE_OutSample</t>
+          <t>RMSE_TestSample</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>R2_OutSample</t>
+          <t>R2_TestSample</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Adjusted_R2_OutSample</t>
+          <t>Adjusted_R2_TestSample</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -499,13 +499,13 @@
         <v>0.6530383496162184</v>
       </c>
       <c r="E2" t="n">
-        <v>1.117096587486254</v>
+        <v>0.1801641115658563</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.7077934144991567</v>
+        <v>0.9454294466443746</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.9160609040722245</v>
+        <v>0.9403766176299648</v>
       </c>
       <c r="H2" t="n">
         <v>-34.06924510713176</v>
@@ -531,13 +531,13 @@
         <v>0.6674437150738057</v>
       </c>
       <c r="E3" t="n">
-        <v>1.119446079301532</v>
+        <v>0.1736332819363075</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.7170410906063811</v>
+        <v>0.9510423763266515</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.9745972541973384</v>
+        <v>0.945500003835329</v>
       </c>
       <c r="H3" t="n">
         <v>-11.84597741942612</v>
@@ -563,13 +563,13 @@
         <v>0.7481594347541545</v>
       </c>
       <c r="E4" t="n">
-        <v>1.121769859830732</v>
+        <v>0.1632675558436219</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.7288663917110008</v>
+        <v>0.9556315991925847</v>
       </c>
       <c r="G4" t="n">
-        <v>-1.039175744069385</v>
+        <v>0.9496589298531249</v>
       </c>
       <c r="H4" t="n">
         <v>14.78899044842026</v>
@@ -595,13 +595,13 @@
         <v>0.7545786023983512</v>
       </c>
       <c r="E5" t="n">
-        <v>1.123010048774031</v>
+        <v>0.1542706850041704</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.7310235383766446</v>
+        <v>0.9625584272765664</v>
       </c>
       <c r="G5" t="n">
-        <v>-1.095449546455938</v>
+        <v>0.9566852393983807</v>
       </c>
       <c r="H5" t="n">
         <v>35.32883616439746</v>
@@ -627,13 +627,13 @@
         <v>0.7606450391778863</v>
       </c>
       <c r="E6" t="n">
-        <v>1.124355118554229</v>
+        <v>0.1469574528607001</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.7347056719568765</v>
+        <v>0.9674561806886989</v>
       </c>
       <c r="G6" t="n">
-        <v>-1.156661105676117</v>
+        <v>0.9615982932126647</v>
       </c>
       <c r="H6" t="n">
         <v>59.7188430879205</v>
@@ -659,13 +659,13 @@
         <v>0.7663841720060641</v>
       </c>
       <c r="E7" t="n">
-        <v>1.125583297310352</v>
+        <v>0.1391661125983226</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.7391441524492126</v>
+        <v>0.9712112835033809</v>
       </c>
       <c r="G7" t="n">
-        <v>-1.222239750351771</v>
+        <v>0.9653360352387648</v>
       </c>
       <c r="H7" t="n">
         <v>84.17233571028811</v>
@@ -691,13 +691,13 @@
         <v>0.7709634214465004</v>
       </c>
       <c r="E8" t="n">
-        <v>1.127362976504438</v>
+        <v>0.1318358622157212</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.743862431541843</v>
+        <v>0.9743259144451667</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.291933481454993</v>
+        <v>0.9684422698388507</v>
       </c>
       <c r="H8" t="n">
         <v>104.6706067561827</v>
@@ -723,13 +723,13 @@
         <v>0.7757482819534524</v>
       </c>
       <c r="E9" t="n">
-        <v>1.127936732564451</v>
+        <v>0.1266954201762954</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.7454182841712962</v>
+        <v>0.976879555937572</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.361448266819989</v>
+        <v>0.9709764638365266</v>
       </c>
       <c r="H9" t="n">
         <v>120.9616187336086</v>

</xml_diff>